<commit_message>
update redirects after successful ad change. update for ad edit
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Softuni\Angular\Angular-Exam-Project\SoftUni-AngularJS-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server\WebstormProjects\SoftUni-AngularJS-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,9 @@
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -986,7 +988,9 @@
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1228,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
edit inactive ads complete
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server\WebstormProjects\SoftUni-AngularJS-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Softuni\Angular\Angular-Exam-Project\SoftUni-AngularJS-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +968,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -978,7 +980,9 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1232,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>